<commit_message>
New: Drug cases by state
</commit_message>
<xml_diff>
--- a/2024-02-10_cny/src.xlsx
+++ b/2024-02-10_cny/src.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10119"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/theveshtheva/git-thevesh/charts/src/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/theveshtheva/git-thevesh/charts/2024-02-10_cny/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33C491E6-F163-2149-8DBD-69989383BD02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD4771F5-1AC6-A442-AC6C-08056253791E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4680" yWindow="500" windowWidth="33720" windowHeight="21100" xr2:uid="{0F32D373-AA13-E844-A237-46170FFDB5EE}"/>
+    <workbookView xWindow="4680" yWindow="500" windowWidth="33720" windowHeight="21100" activeTab="1" xr2:uid="{0F32D373-AA13-E844-A237-46170FFDB5EE}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="annual" sheetId="1" r:id="rId1"/>
+    <sheet name="qtr" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
@@ -36,12 +37,36 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
   <si>
     <t>year</t>
   </si>
   <si>
     <t>births</t>
+  </si>
+  <si>
+    <t>Q1</t>
+  </si>
+  <si>
+    <t>Q2</t>
+  </si>
+  <si>
+    <t>Q3</t>
+  </si>
+  <si>
+    <t>Q4</t>
+  </si>
+  <si>
+    <t>2023a</t>
+  </si>
+  <si>
+    <t>2023f</t>
+  </si>
+  <si>
+    <t>2024a</t>
+  </si>
+  <si>
+    <t>2022f</t>
   </si>
 </sst>
 </file>
@@ -113,9 +138,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -153,7 +178,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -259,7 +284,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -401,7 +426,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -411,7 +436,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8DB7AA7-813F-B047-BD68-B52C4A4B42CA}">
   <dimension ref="A1:Q33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -837,4 +862,101 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B197F31-E032-E94B-8E52-4743D0927E97}">
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2">
+        <v>9112</v>
+      </c>
+      <c r="C2">
+        <v>8335</v>
+      </c>
+      <c r="D2">
+        <v>10985</v>
+      </c>
+      <c r="E2">
+        <v>11884</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3">
+        <v>9892</v>
+      </c>
+      <c r="C3">
+        <v>9596</v>
+      </c>
+      <c r="D3">
+        <v>9930</v>
+      </c>
+      <c r="E3">
+        <v>10525</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4">
+        <v>11434</v>
+      </c>
+      <c r="C4">
+        <v>11077</v>
+      </c>
+      <c r="D4">
+        <v>11162</v>
+      </c>
+      <c r="E4">
+        <v>11145</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5">
+        <v>9372</v>
+      </c>
+      <c r="C5">
+        <v>9786</v>
+      </c>
+      <c r="D5">
+        <v>10427</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>